<commit_message>
code added for verifying 4 values.
</commit_message>
<xml_diff>
--- a/fox.webautomation.com/src/test/resources/Test.xlsx
+++ b/fox.webautomation.com/src/test/resources/Test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10645475\Desktop\fox.webautomation.com\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10645475\git\repository2\fox.webautomation.com\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86BD1EB-D0F8-40F5-B621-68DB2D878799}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60530EB-B6CF-4719-B861-9501FC702283}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-119" yWindow="-119" windowWidth="19240" windowHeight="14846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>TestName</t>
   </si>
@@ -74,37 +74,34 @@
     <t>TestData14</t>
   </si>
   <si>
-    <t>Sick</t>
-  </si>
-  <si>
-    <t>9608.70 - Police Department - Studio: Guards-001</t>
-  </si>
-  <si>
-    <t>Awaiting Approval</t>
-  </si>
-  <si>
-    <t>01/30/2020 - 01/30/2020</t>
-  </si>
-  <si>
-    <t>01/30/2020</t>
-  </si>
-  <si>
     <t>test_tour_revenue</t>
   </si>
   <si>
-    <t>test_click_tour_revenue</t>
-  </si>
-  <si>
     <t>test_tour_inventory</t>
   </si>
   <si>
     <t>test_target_audience_builder</t>
+  </si>
+  <si>
+    <t>test_tour_cashweekly</t>
+  </si>
+  <si>
+    <t>$4,279.8</t>
+  </si>
+  <si>
+    <t>$53.2</t>
+  </si>
+  <si>
+    <t>$658.7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -144,6 +141,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,12 +427,12 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
@@ -498,44 +498,32 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="3"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -546,7 +534,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -557,7 +545,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>

</xml_diff>